<commit_message>
feat: add xlsx demo page add export of simple-table page
</commit_message>
<xml_diff>
--- a/src/assets/demo.xlsx
+++ b/src/assets/demo.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asdf\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asdf\Desktop\work\delon\scaffold\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,6 +21,29 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>编号</t>
+  </si>
+  <si>
+    <t>姓名</t>
+  </si>
+  <si>
+    <t>年龄</t>
+  </si>
+  <si>
+    <t>注册日期</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>cipchk</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -54,8 +77,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -370,12 +394,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>26</v>
+      </c>
+      <c r="D3" s="1">
+        <v>43101</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>